<commit_message>
Delete "new" and unused import
</commit_message>
<xml_diff>
--- a/docs/GrilleNotation.xlsx
+++ b/docs/GrilleNotation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/91eae10498081058/Documents/^N^N^N/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/91eae10498081058/Documents/Safran/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="690" documentId="13_ncr:1_{E138E7C9-009E-4D59-A9DA-AA9F4A5AA8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FB81123-EF91-4C12-923C-6BD84ACAA4D4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{AB6F6693-6B8C-4684-9576-BC4DD09BE9E0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{AB6F6693-6B8C-4684-9576-BC4DD09BE9E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Grille Eval Bloc1" sheetId="2" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Grille Eval Bloc1'!$A$1:$F$25</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1275,6 +1276,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1314,41 +1321,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1641,10 +1642,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1949,44 +1946,44 @@
   </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="70.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="70.5546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.77734375" style="1"/>
+    <col min="1" max="1" width="17.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="70.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="70.5703125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.4">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="63"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="62" t="s">
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A2" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="64"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="66"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="15"/>
@@ -1994,30 +1991,30 @@
       <c r="E3" s="16"/>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="65" t="s">
+    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="67" t="s">
+      <c r="B4" s="68"/>
+      <c r="C4" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="70"/>
       <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="65" t="s">
+    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="67" t="s">
+      <c r="B5" s="68"/>
+      <c r="C5" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="68"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D5" s="70"/>
+    </row>
+    <row r="6" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -2025,7 +2022,7 @@
       <c r="E6" s="13"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:7" s="30" customFormat="1" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="30" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
@@ -2046,25 +2043,25 @@
       </c>
       <c r="G7" s="29"/>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="56" t="s">
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="58" t="s">
         <v>131</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="80" t="s">
+      <c r="D8" s="57" t="s">
         <v>134</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="19"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="105.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="57"/>
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="105.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="59"/>
       <c r="B9" s="17" t="s">
         <v>27</v>
       </c>
@@ -2078,8 +2075,8 @@
       <c r="F9" s="19"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" ht="112.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="57"/>
+    <row r="10" spans="1:7" s="5" customFormat="1" ht="112.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="59"/>
       <c r="B10" s="17" t="s">
         <v>29</v>
       </c>
@@ -2093,8 +2090,8 @@
       <c r="F10" s="19"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" s="5" customFormat="1" ht="151.19999999999999" x14ac:dyDescent="0.3">
-      <c r="A11" s="57"/>
+    <row r="11" spans="1:7" s="5" customFormat="1" ht="117" x14ac:dyDescent="0.25">
+      <c r="A11" s="59"/>
       <c r="B11" s="17" t="s">
         <v>32</v>
       </c>
@@ -2108,8 +2105,8 @@
       <c r="F11" s="19"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="57"/>
+    <row r="12" spans="1:7" s="5" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="59"/>
       <c r="B12" s="17" t="s">
         <v>35</v>
       </c>
@@ -2123,8 +2120,8 @@
       <c r="F12" s="19"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" s="5" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="57"/>
+    <row r="13" spans="1:7" s="5" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="59"/>
       <c r="B13" s="17" t="s">
         <v>38</v>
       </c>
@@ -2138,8 +2135,8 @@
       <c r="F13" s="19"/>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7" s="5" customFormat="1" ht="128.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="57"/>
+    <row r="14" spans="1:7" s="5" customFormat="1" ht="128.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="59"/>
       <c r="B14" s="17" t="s">
         <v>41</v>
       </c>
@@ -2153,8 +2150,8 @@
       <c r="F14" s="19"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" ht="120.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="57"/>
+    <row r="15" spans="1:7" s="5" customFormat="1" ht="120.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="59"/>
       <c r="B15" s="17" t="s">
         <v>44</v>
       </c>
@@ -2168,8 +2165,8 @@
       <c r="F15" s="19"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" ht="100.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="57"/>
+    <row r="16" spans="1:7" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="59"/>
       <c r="B16" s="17" t="s">
         <v>47</v>
       </c>
@@ -2183,8 +2180,8 @@
       <c r="F16" s="20"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" ht="183.6" x14ac:dyDescent="0.35">
-      <c r="A17" s="57"/>
+    <row r="17" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A17" s="59"/>
       <c r="B17" s="45" t="s">
         <v>50</v>
       </c>
@@ -2198,8 +2195,8 @@
       <c r="F17" s="46"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" ht="94.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="58"/>
+    <row r="18" spans="1:7" ht="94.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="60"/>
       <c r="B18" s="21" t="s">
         <v>53</v>
       </c>
@@ -2213,7 +2210,7 @@
       <c r="F18" s="23"/>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" ht="14.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="14.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -2223,12 +2220,12 @@
       </c>
       <c r="F19" s="14"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>13</v>
       </c>
@@ -2241,7 +2238,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
@@ -2254,7 +2251,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="34" t="s">
         <v>15</v>
       </c>
@@ -2298,40 +2295,40 @@
       <selection activeCell="A8" sqref="A8:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.21875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="70.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="70.5546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.77734375" style="1"/>
+    <col min="1" max="1" width="19.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="70.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="70.5703125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.4">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="63"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="62" t="s">
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A2" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="64"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="66"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="15"/>
@@ -2339,30 +2336,30 @@
       <c r="E3" s="16"/>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="65" t="s">
+    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="67" t="s">
+      <c r="B4" s="68"/>
+      <c r="C4" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="70"/>
       <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="65" t="s">
+    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="67" t="s">
+      <c r="B5" s="68"/>
+      <c r="C5" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="68"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D5" s="70"/>
+    </row>
+    <row r="6" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -2370,7 +2367,7 @@
       <c r="E6" s="13"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:7" s="30" customFormat="1" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="30" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
@@ -2391,8 +2388,8 @@
       </c>
       <c r="G7" s="29"/>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="154.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="56"/>
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="154.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="58"/>
       <c r="B8" s="17" t="s">
         <v>57</v>
       </c>
@@ -2406,8 +2403,8 @@
       <c r="F8" s="19"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="64.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="57"/>
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="59"/>
       <c r="B9" s="17" t="s">
         <v>60</v>
       </c>
@@ -2421,8 +2418,8 @@
       <c r="F9" s="19"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" ht="146.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="57"/>
+    <row r="10" spans="1:7" s="5" customFormat="1" ht="146.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="59"/>
       <c r="B10" s="17" t="s">
         <v>63</v>
       </c>
@@ -2436,8 +2433,8 @@
       <c r="F10" s="19"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="57"/>
+    <row r="11" spans="1:7" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A11" s="59"/>
       <c r="B11" s="17" t="s">
         <v>66</v>
       </c>
@@ -2451,8 +2448,8 @@
       <c r="F11" s="19"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" ht="92.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="57"/>
+    <row r="12" spans="1:7" s="5" customFormat="1" ht="92.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="59"/>
       <c r="B12" s="17" t="s">
         <v>69</v>
       </c>
@@ -2466,8 +2463,8 @@
       <c r="F12" s="19"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" s="5" customFormat="1" ht="79.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="57"/>
+    <row r="13" spans="1:7" s="5" customFormat="1" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="59"/>
       <c r="B13" s="17" t="s">
         <v>72</v>
       </c>
@@ -2481,8 +2478,8 @@
       <c r="F13" s="19"/>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7" s="5" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="57"/>
+    <row r="14" spans="1:7" s="5" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="59"/>
       <c r="B14" s="17" t="s">
         <v>75</v>
       </c>
@@ -2496,8 +2493,8 @@
       <c r="F14" s="19"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="57"/>
+    <row r="15" spans="1:7" s="5" customFormat="1" ht="91.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="59"/>
       <c r="B15" s="17" t="s">
         <v>78</v>
       </c>
@@ -2511,8 +2508,8 @@
       <c r="F15" s="19"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="58"/>
+    <row r="16" spans="1:7" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="60"/>
       <c r="B16" s="21" t="s">
         <v>81</v>
       </c>
@@ -2526,7 +2523,7 @@
       <c r="F16" s="23"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:6" ht="14.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="14.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -2536,12 +2533,12 @@
       </c>
       <c r="F17" s="14"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>13</v>
       </c>
@@ -2554,7 +2551,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>14</v>
       </c>
@@ -2567,7 +2564,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="34" t="s">
         <v>15</v>
       </c>
@@ -2611,40 +2608,40 @@
       <selection activeCell="A8" sqref="A8:A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="70.5546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.77734375" style="1"/>
+    <col min="2" max="2" width="38.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="70.5703125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.4">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="63"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="62" t="s">
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A2" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="64"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="66"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="15"/>
@@ -2652,30 +2649,30 @@
       <c r="E3" s="16"/>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="65" t="s">
+    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="67" t="s">
+      <c r="B4" s="68"/>
+      <c r="C4" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="70"/>
       <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="65" t="s">
+    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="67" t="s">
+      <c r="B5" s="68"/>
+      <c r="C5" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="68"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D5" s="70"/>
+    </row>
+    <row r="6" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -2683,7 +2680,7 @@
       <c r="E6" s="13"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:7" s="30" customFormat="1" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="30" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
@@ -2704,8 +2701,8 @@
       </c>
       <c r="G7" s="29"/>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="186" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="56" t="s">
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="186" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="58" t="s">
         <v>84</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -2721,8 +2718,8 @@
       <c r="F8" s="19"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="57"/>
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="59"/>
       <c r="B9" s="17" t="s">
         <v>88</v>
       </c>
@@ -2736,8 +2733,8 @@
       <c r="F9" s="19"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" ht="83.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="57"/>
+    <row r="10" spans="1:7" s="5" customFormat="1" ht="83.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="59"/>
       <c r="B10" s="17" t="s">
         <v>91</v>
       </c>
@@ -2751,8 +2748,8 @@
       <c r="F10" s="19"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" s="5" customFormat="1" ht="223.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="57"/>
+    <row r="11" spans="1:7" s="5" customFormat="1" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="59"/>
       <c r="B11" s="17" t="s">
         <v>94</v>
       </c>
@@ -2766,8 +2763,8 @@
       <c r="F11" s="19"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" ht="150.44999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="57"/>
+    <row r="12" spans="1:7" s="5" customFormat="1" ht="150.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="59"/>
       <c r="B12" s="17" t="s">
         <v>97</v>
       </c>
@@ -2781,8 +2778,8 @@
       <c r="F12" s="19"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" s="5" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="57"/>
+    <row r="13" spans="1:7" s="5" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="59"/>
       <c r="B13" s="17" t="s">
         <v>100</v>
       </c>
@@ -2796,8 +2793,8 @@
       <c r="F13" s="19"/>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7" ht="103.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="58"/>
+    <row r="14" spans="1:7" ht="103.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="60"/>
       <c r="B14" s="21" t="s">
         <v>103</v>
       </c>
@@ -2811,7 +2808,7 @@
       <c r="F14" s="23"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" ht="14.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="14.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31"/>
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
@@ -2821,12 +2818,12 @@
       </c>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>13</v>
       </c>
@@ -2839,7 +2836,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>14</v>
       </c>
@@ -2852,7 +2849,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="34" t="s">
         <v>15</v>
       </c>
@@ -2896,40 +2893,40 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="70.5546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.77734375" style="1"/>
+    <col min="2" max="2" width="38.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="70.5703125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.4">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="63"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="62" t="s">
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A2" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="64"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="66"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="15"/>
@@ -2937,30 +2934,30 @@
       <c r="E3" s="16"/>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="65" t="s">
+    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="67" t="s">
+      <c r="B4" s="68"/>
+      <c r="C4" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="70"/>
       <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="65" t="s">
+    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="67" t="s">
+      <c r="B5" s="68"/>
+      <c r="C5" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="68"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D5" s="70"/>
+    </row>
+    <row r="6" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -2968,7 +2965,7 @@
       <c r="E6" s="13"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:7" s="30" customFormat="1" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="30" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
@@ -2989,8 +2986,8 @@
       </c>
       <c r="G7" s="29"/>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="73.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="56" t="s">
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="58" t="s">
         <v>132</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -3006,8 +3003,8 @@
       <c r="F8" s="19"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="112.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="57"/>
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="112.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="59"/>
       <c r="B9" s="17" t="s">
         <v>110</v>
       </c>
@@ -3021,8 +3018,8 @@
       <c r="F9" s="19"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" ht="112.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="57"/>
+    <row r="10" spans="1:7" s="5" customFormat="1" ht="112.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="59"/>
       <c r="B10" s="17" t="s">
         <v>113</v>
       </c>
@@ -3036,8 +3033,8 @@
       <c r="F10" s="19"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" s="5" customFormat="1" ht="65.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="57"/>
+    <row r="11" spans="1:7" s="5" customFormat="1" ht="65.650000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="59"/>
       <c r="B11" s="17" t="s">
         <v>116</v>
       </c>
@@ -3051,8 +3048,8 @@
       <c r="F11" s="19"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" ht="75.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="57"/>
+    <row r="12" spans="1:7" s="5" customFormat="1" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="59"/>
       <c r="B12" s="17" t="s">
         <v>119</v>
       </c>
@@ -3066,8 +3063,8 @@
       <c r="F12" s="19"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" s="5" customFormat="1" ht="60.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="57"/>
+    <row r="13" spans="1:7" s="5" customFormat="1" ht="60.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="59"/>
       <c r="B13" s="17" t="s">
         <v>122</v>
       </c>
@@ -3081,8 +3078,8 @@
       <c r="F13" s="19"/>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7" s="5" customFormat="1" ht="60.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="58"/>
+    <row r="14" spans="1:7" s="5" customFormat="1" ht="60.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="60"/>
       <c r="B14" s="21" t="s">
         <v>125</v>
       </c>
@@ -3096,7 +3093,7 @@
       <c r="F14" s="54"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" ht="14.55" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="14.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31"/>
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
@@ -3106,12 +3103,12 @@
       </c>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>13</v>
       </c>
@@ -3124,7 +3121,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>14</v>
       </c>
@@ -3137,7 +3134,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="34" t="s">
         <v>15</v>
       </c>
@@ -3177,46 +3174,46 @@
   </sheetPr>
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" style="1" customWidth="1"/>
     <col min="2" max="2" width="65" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" style="39" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" style="1" customWidth="1"/>
-    <col min="5" max="6" width="20.5546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="70.5546875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.77734375" style="1"/>
+    <col min="3" max="3" width="11.7109375" style="39" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="20.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="70.5703125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.4">
+      <c r="A1" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="63"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="62" t="s">
+    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A2" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="64"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="66"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="6"/>
@@ -3225,32 +3222,32 @@
       <c r="F3" s="16"/>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="65" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="67" t="s">
+      <c r="B4" s="68"/>
+      <c r="C4" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="68"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="70"/>
       <c r="G4" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="65" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="67" t="s">
+      <c r="B5" s="68"/>
+      <c r="C5" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="76"/>
-      <c r="E5" s="68"/>
-    </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D5" s="73"/>
+      <c r="E5" s="70"/>
+    </row>
+    <row r="6" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="4"/>
@@ -3259,7 +3256,7 @@
       <c r="F6" s="13"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:8" s="30" customFormat="1" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="30" customFormat="1" ht="41.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
@@ -3283,8 +3280,8 @@
       </c>
       <c r="H7" s="29"/>
     </row>
-    <row r="8" spans="1:8" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="56" t="s">
+    <row r="8" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A8" s="58" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -3294,13 +3291,13 @@
         <v>128</v>
       </c>
       <c r="D8" s="38"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="77"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="75"/>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="57"/>
+    <row r="9" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A9" s="59"/>
       <c r="B9" s="17" t="s">
         <v>27</v>
       </c>
@@ -3308,13 +3305,13 @@
         <v>129</v>
       </c>
       <c r="D9" s="38"/>
-      <c r="E9" s="70"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="74"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="77"/>
+      <c r="G9" s="72"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:8" s="5" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="57"/>
+    <row r="10" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="59"/>
       <c r="B10" s="17" t="s">
         <v>29</v>
       </c>
@@ -3322,13 +3319,13 @@
         <v>129</v>
       </c>
       <c r="D10" s="38"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="74"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="72"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="57"/>
+    <row r="11" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A11" s="59"/>
       <c r="B11" s="17" t="s">
         <v>32</v>
       </c>
@@ -3336,13 +3333,13 @@
         <v>128</v>
       </c>
       <c r="D11" s="38"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="74"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="72"/>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="57"/>
+    <row r="12" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A12" s="59"/>
       <c r="B12" s="17" t="s">
         <v>35</v>
       </c>
@@ -3350,13 +3347,13 @@
         <v>129</v>
       </c>
       <c r="D12" s="38"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="74"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="72"/>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="57"/>
+    <row r="13" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A13" s="59"/>
       <c r="B13" s="17" t="s">
         <v>38</v>
       </c>
@@ -3364,13 +3361,13 @@
         <v>129</v>
       </c>
       <c r="D13" s="38"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="74"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="72"/>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="57"/>
+    <row r="14" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A14" s="59"/>
       <c r="B14" s="17" t="s">
         <v>41</v>
       </c>
@@ -3378,13 +3375,13 @@
         <v>128</v>
       </c>
       <c r="D14" s="38"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="74"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="72"/>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="57"/>
+    <row r="15" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="59"/>
       <c r="B15" s="17" t="s">
         <v>44</v>
       </c>
@@ -3392,13 +3389,13 @@
         <v>128</v>
       </c>
       <c r="D15" s="38"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="74"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="72"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="57"/>
+    <row r="16" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="59"/>
       <c r="B16" s="17" t="s">
         <v>47</v>
       </c>
@@ -3406,13 +3403,13 @@
         <v>129</v>
       </c>
       <c r="D16" s="38"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="74"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="72"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="57"/>
+    <row r="17" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A17" s="59"/>
       <c r="B17" s="17" t="s">
         <v>50</v>
       </c>
@@ -3420,13 +3417,13 @@
         <v>129</v>
       </c>
       <c r="D17" s="38"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="74"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="72"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="1:8" s="5" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="58"/>
+    <row r="18" spans="1:8" s="5" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="60"/>
       <c r="B18" s="21" t="s">
         <v>53</v>
       </c>
@@ -3434,13 +3431,13 @@
         <v>128</v>
       </c>
       <c r="D18" s="36"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="74"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="77"/>
+      <c r="G18" s="72"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" ht="33" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="72" t="s">
+    <row r="19" spans="1:8" s="5" customFormat="1" ht="18.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="74" t="s">
         <v>56</v>
       </c>
       <c r="B19" s="42" t="s">
@@ -3450,13 +3447,13 @@
         <v>129</v>
       </c>
       <c r="D19" s="43"/>
-      <c r="E19" s="69"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="73"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="71"/>
       <c r="H19" s="9"/>
     </row>
-    <row r="20" spans="1:8" s="5" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="57"/>
+    <row r="20" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A20" s="59"/>
       <c r="B20" s="47" t="s">
         <v>60</v>
       </c>
@@ -3464,13 +3461,13 @@
         <v>129</v>
       </c>
       <c r="D20" s="48"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="74"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="72"/>
       <c r="H20" s="9"/>
     </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="57"/>
+    <row r="21" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A21" s="59"/>
       <c r="B21" s="47" t="s">
         <v>63</v>
       </c>
@@ -3478,13 +3475,13 @@
         <v>128</v>
       </c>
       <c r="D21" s="48"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="74"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="72"/>
       <c r="H21" s="9"/>
     </row>
-    <row r="22" spans="1:8" s="5" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="57"/>
+    <row r="22" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="59"/>
       <c r="B22" s="47" t="s">
         <v>66</v>
       </c>
@@ -3492,13 +3489,13 @@
         <v>128</v>
       </c>
       <c r="D22" s="48"/>
-      <c r="E22" s="70"/>
-      <c r="F22" s="70"/>
-      <c r="G22" s="74"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="72"/>
       <c r="H22" s="9"/>
     </row>
-    <row r="23" spans="1:8" s="5" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="57"/>
+    <row r="23" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A23" s="59"/>
       <c r="B23" s="47" t="s">
         <v>69</v>
       </c>
@@ -3506,13 +3503,13 @@
         <v>128</v>
       </c>
       <c r="D23" s="48"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="74"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="72"/>
       <c r="H23" s="9"/>
     </row>
-    <row r="24" spans="1:8" s="5" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="57"/>
+    <row r="24" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A24" s="59"/>
       <c r="B24" s="47" t="s">
         <v>72</v>
       </c>
@@ -3520,13 +3517,13 @@
         <v>129</v>
       </c>
       <c r="D24" s="48"/>
-      <c r="E24" s="70"/>
-      <c r="F24" s="70"/>
-      <c r="G24" s="74"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="72"/>
       <c r="H24" s="9"/>
     </row>
-    <row r="25" spans="1:8" s="5" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="57"/>
+    <row r="25" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="59"/>
       <c r="B25" s="47" t="s">
         <v>75</v>
       </c>
@@ -3534,13 +3531,13 @@
         <v>128</v>
       </c>
       <c r="D25" s="48"/>
-      <c r="E25" s="70"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="74"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="72"/>
       <c r="H25" s="9"/>
     </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="57"/>
+    <row r="26" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="59"/>
       <c r="B26" s="17" t="s">
         <v>78</v>
       </c>
@@ -3548,13 +3545,13 @@
         <v>129</v>
       </c>
       <c r="D26" s="38"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="74"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="72"/>
       <c r="H26" s="9"/>
     </row>
-    <row r="27" spans="1:8" s="5" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="58"/>
+    <row r="27" spans="1:8" s="5" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="60"/>
       <c r="B27" s="21" t="s">
         <v>81</v>
       </c>
@@ -3562,13 +3559,13 @@
         <v>129</v>
       </c>
       <c r="D27" s="36"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="74"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="72"/>
       <c r="H27" s="9"/>
     </row>
-    <row r="28" spans="1:8" s="5" customFormat="1" ht="33" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="72" t="s">
+    <row r="28" spans="1:8" s="5" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="74" t="s">
         <v>84</v>
       </c>
       <c r="B28" s="42" t="s">
@@ -3578,13 +3575,13 @@
         <v>128</v>
       </c>
       <c r="D28" s="43"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="69"/>
-      <c r="G28" s="73"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="71"/>
       <c r="H28" s="9"/>
     </row>
-    <row r="29" spans="1:8" s="5" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="57"/>
+    <row r="29" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A29" s="59"/>
       <c r="B29" s="17" t="s">
         <v>88</v>
       </c>
@@ -3592,13 +3589,13 @@
         <v>128</v>
       </c>
       <c r="D29" s="38"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="74"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="72"/>
       <c r="H29" s="9"/>
     </row>
-    <row r="30" spans="1:8" s="5" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="57"/>
+    <row r="30" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="59"/>
       <c r="B30" s="17" t="s">
         <v>91</v>
       </c>
@@ -3606,13 +3603,13 @@
         <v>129</v>
       </c>
       <c r="D30" s="38"/>
-      <c r="E30" s="70"/>
-      <c r="F30" s="70"/>
-      <c r="G30" s="74"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="72"/>
       <c r="H30" s="9"/>
     </row>
-    <row r="31" spans="1:8" s="5" customFormat="1" ht="54" x14ac:dyDescent="0.3">
-      <c r="A31" s="57"/>
+    <row r="31" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A31" s="59"/>
       <c r="B31" s="17" t="s">
         <v>94</v>
       </c>
@@ -3620,13 +3617,13 @@
         <v>129</v>
       </c>
       <c r="D31" s="38"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="74"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="72"/>
       <c r="H31" s="9"/>
     </row>
-    <row r="32" spans="1:8" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="57"/>
+    <row r="32" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A32" s="59"/>
       <c r="B32" s="17" t="s">
         <v>97</v>
       </c>
@@ -3634,13 +3631,13 @@
         <v>129</v>
       </c>
       <c r="D32" s="38"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="70"/>
-      <c r="G32" s="74"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="72"/>
       <c r="H32" s="9"/>
     </row>
-    <row r="33" spans="1:8" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="57"/>
+    <row r="33" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A33" s="59"/>
       <c r="B33" s="17" t="s">
         <v>100</v>
       </c>
@@ -3648,13 +3645,13 @@
         <v>129</v>
       </c>
       <c r="D33" s="38"/>
-      <c r="E33" s="70"/>
-      <c r="F33" s="70"/>
-      <c r="G33" s="74"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="72"/>
       <c r="H33" s="9"/>
     </row>
-    <row r="34" spans="1:8" s="5" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="57"/>
+    <row r="34" spans="1:8" s="5" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="59"/>
       <c r="B34" s="21" t="s">
         <v>103</v>
       </c>
@@ -3662,13 +3659,13 @@
         <v>128</v>
       </c>
       <c r="D34" s="38"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="74"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="77"/>
+      <c r="G34" s="72"/>
       <c r="H34" s="9"/>
     </row>
-    <row r="35" spans="1:8" s="5" customFormat="1" ht="33" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="72" t="s">
+    <row r="35" spans="1:8" s="5" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="74" t="s">
         <v>106</v>
       </c>
       <c r="B35" s="42" t="s">
@@ -3678,13 +3675,13 @@
         <v>129</v>
       </c>
       <c r="D35" s="43"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="73"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="78"/>
+      <c r="G35" s="71"/>
       <c r="H35" s="9"/>
     </row>
-    <row r="36" spans="1:8" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="57"/>
+    <row r="36" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A36" s="59"/>
       <c r="B36" s="17" t="s">
         <v>110</v>
       </c>
@@ -3692,13 +3689,13 @@
         <v>128</v>
       </c>
       <c r="D36" s="38"/>
-      <c r="E36" s="70"/>
-      <c r="F36" s="70"/>
-      <c r="G36" s="74"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="77"/>
+      <c r="G36" s="72"/>
       <c r="H36" s="9"/>
     </row>
-    <row r="37" spans="1:8" s="5" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="57"/>
+    <row r="37" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A37" s="59"/>
       <c r="B37" s="17" t="s">
         <v>113</v>
       </c>
@@ -3706,13 +3703,13 @@
         <v>128</v>
       </c>
       <c r="D37" s="38"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="74"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="77"/>
+      <c r="G37" s="72"/>
       <c r="H37" s="9"/>
     </row>
-    <row r="38" spans="1:8" s="5" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="57"/>
+    <row r="38" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A38" s="59"/>
       <c r="B38" s="17" t="s">
         <v>116</v>
       </c>
@@ -3720,13 +3717,13 @@
         <v>129</v>
       </c>
       <c r="D38" s="38"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="70"/>
-      <c r="G38" s="74"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="77"/>
+      <c r="G38" s="72"/>
       <c r="H38" s="9"/>
     </row>
-    <row r="39" spans="1:8" s="5" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="57"/>
+    <row r="39" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A39" s="59"/>
       <c r="B39" s="17" t="s">
         <v>119</v>
       </c>
@@ -3734,13 +3731,13 @@
         <v>129</v>
       </c>
       <c r="D39" s="38"/>
-      <c r="E39" s="70"/>
-      <c r="F39" s="70"/>
-      <c r="G39" s="74"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="72"/>
       <c r="H39" s="9"/>
     </row>
-    <row r="40" spans="1:8" s="5" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="57"/>
+    <row r="40" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A40" s="59"/>
       <c r="B40" s="17" t="s">
         <v>122</v>
       </c>
@@ -3748,13 +3745,13 @@
         <v>128</v>
       </c>
       <c r="D40" s="38"/>
-      <c r="E40" s="70"/>
-      <c r="F40" s="70"/>
-      <c r="G40" s="74"/>
+      <c r="E40" s="77"/>
+      <c r="F40" s="77"/>
+      <c r="G40" s="72"/>
       <c r="H40" s="9"/>
     </row>
-    <row r="41" spans="1:8" s="5" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="58"/>
+    <row r="41" spans="1:8" s="5" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="60"/>
       <c r="B41" s="21" t="s">
         <v>125</v>
       </c>
@@ -3762,12 +3759,12 @@
         <v>129</v>
       </c>
       <c r="D41" s="36"/>
-      <c r="E41" s="71"/>
-      <c r="F41" s="71"/>
-      <c r="G41" s="75"/>
+      <c r="E41" s="79"/>
+      <c r="F41" s="79"/>
+      <c r="G41" s="80"/>
       <c r="H41" s="9"/>
     </row>
-    <row r="42" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A42" s="14"/>
       <c r="B42" s="14"/>
       <c r="C42" s="6"/>
@@ -3776,7 +3773,7 @@
       <c r="F42" s="16"/>
       <c r="G42" s="14"/>
     </row>
-    <row r="43" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="E43" s="40" t="s">
         <v>23</v>
       </c>
@@ -3784,6 +3781,13 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="F35:F41"/>
+    <mergeCell ref="E35:E41"/>
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="A35:A41"/>
+    <mergeCell ref="G35:G41"/>
+    <mergeCell ref="F28:F34"/>
+    <mergeCell ref="E28:E34"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A4:B4"/>
@@ -3799,13 +3803,6 @@
     <mergeCell ref="E8:E18"/>
     <mergeCell ref="F19:F27"/>
     <mergeCell ref="E19:E27"/>
-    <mergeCell ref="F35:F41"/>
-    <mergeCell ref="E35:E41"/>
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="A35:A41"/>
-    <mergeCell ref="G35:G41"/>
-    <mergeCell ref="F28:F34"/>
-    <mergeCell ref="E28:E34"/>
   </mergeCells>
   <conditionalFormatting sqref="F43">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
@@ -3837,6 +3834,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="1ba08013-ef1c-4130-a497-bc53eb55e168" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ed22885-9a1c-4a78-8ce9-dd4492997226">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010097798227B93F3B46A4C8EE6693783472" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="07a0dc2af2640077c1870da1684932dd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1ba08013-ef1c-4130-a497-bc53eb55e168" xmlns:ns3="0ed22885-9a1c-4a78-8ce9-dd4492997226" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9f8b351a6a60032acdf3e22257ff17f6" ns2:_="" ns3:_="">
     <xsd:import namespace="1ba08013-ef1c-4130-a497-bc53eb55e168"/>
@@ -4065,17 +4073,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="1ba08013-ef1c-4130-a497-bc53eb55e168" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ed22885-9a1c-4a78-8ce9-dd4492997226">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4086,6 +4083,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6771D95-FB55-4106-9918-F95569952A80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="81d943eb-53de-4d5a-93c5-961cb00f222e"/>
+    <ds:schemaRef ds:uri="11399b42-56c9-44ff-9016-8ae70501af32"/>
+    <ds:schemaRef ds:uri="1ba08013-ef1c-4130-a497-bc53eb55e168"/>
+    <ds:schemaRef ds:uri="0ed22885-9a1c-4a78-8ce9-dd4492997226"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F45F5A-8870-483A-962A-5D86A18EB9F0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4104,19 +4114,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6771D95-FB55-4106-9918-F95569952A80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="81d943eb-53de-4d5a-93c5-961cb00f222e"/>
-    <ds:schemaRef ds:uri="11399b42-56c9-44ff-9016-8ae70501af32"/>
-    <ds:schemaRef ds:uri="1ba08013-ef1c-4130-a497-bc53eb55e168"/>
-    <ds:schemaRef ds:uri="0ed22885-9a1c-4a78-8ce9-dd4492997226"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{801D0CEA-46D1-40C8-94B1-8478A557036E}">
   <ds:schemaRefs>

</xml_diff>